<commit_message>
Update Requirements - PENTING.xlsx
</commit_message>
<xml_diff>
--- a/docs/System/Requirements - PENTING.xlsx
+++ b/docs/System/Requirements - PENTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>bendahara</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Lom berez</t>
+  </si>
+  <si>
+    <t>Syarat &amp; ketentuan</t>
+  </si>
+  <si>
+    <t>Isinya apa?</t>
   </si>
 </sst>
 </file>
@@ -731,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,9 +1096,13 @@
       </c>
       <c r="D40" s="14"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
+    <row r="41" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="D41" s="14"/>
     </row>
     <row r="42" spans="2:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update tanggal otik (biar sama kayak yg di server) apdet dokumentasi update db yg di server
</commit_message>
<xml_diff>
--- a/docs/System/Requirements - PENTING.xlsx
+++ b/docs/System/Requirements - PENTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>bendahara</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Isinya apa?</t>
+  </si>
+  <si>
+    <t>LINK DONE</t>
   </si>
 </sst>
 </file>
@@ -737,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1070,9 @@
       <c r="C37" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="14"/>
+      <c r="D37" s="14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">

</xml_diff>